<commit_message>
direct electric is dead
</commit_message>
<xml_diff>
--- a/directelectric.xlsx
+++ b/directelectric.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Ссылка на товар</t>
   </si>
@@ -28,10 +28,19 @@
     <t>Краткое Название товара</t>
   </si>
   <si>
+    <t>Описание товара</t>
+  </si>
+  <si>
     <t>Артикул</t>
   </si>
   <si>
     <t>Цена</t>
+  </si>
+  <si>
+    <t>Наличие</t>
+  </si>
+  <si>
+    <t>Размерность(шт, кг, тонна)</t>
   </si>
 </sst>
 </file>
@@ -359,6 +368,15 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>